<commit_message>
faltan Test y HTML
</commit_message>
<xml_diff>
--- a/recuento.xlsx
+++ b/recuento.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claud\Documents\Tareas Varios\CTD\bimestre5\backend\Examen\KOHEN-NATALIA_CAICEDO-CLAUDIO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{471A689F-6D41-4C7F-8014-D849AFA9DDF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D38CE0-6DD1-4977-8087-6AFF8B0282CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33555" yWindow="-9285" windowWidth="15675" windowHeight="13935" activeTab="1" xr2:uid="{0C4BC463-CAA7-431A-8A47-2C47A2575FA9}"/>
+    <workbookView xWindow="38160" yWindow="-10005" windowWidth="17280" windowHeight="15585" activeTab="1" xr2:uid="{0C4BC463-CAA7-431A-8A47-2C47A2575FA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="48">
   <si>
     <t>nombr</t>
   </si>
@@ -117,9 +117,6 @@
     <t>Turno</t>
   </si>
   <si>
-    <t>FALTA</t>
-  </si>
-  <si>
     <t>Domicilio</t>
   </si>
   <si>
@@ -166,9 +163,6 @@
   </si>
   <si>
     <t>test</t>
-  </si>
-  <si>
-    <t>Faltan todos</t>
   </si>
   <si>
     <t>FRONT</t>
@@ -624,7 +618,7 @@
   <dimension ref="A3:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="F3" sqref="F3:F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -662,7 +656,7 @@
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>21</v>
@@ -673,7 +667,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>15</v>
@@ -728,17 +722,17 @@
         <v>24</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>17</v>
@@ -748,7 +742,7 @@
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>17</v>
@@ -758,7 +752,7 @@
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>17</v>
@@ -767,7 +761,7 @@
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>15</v>
@@ -798,10 +792,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>17</v>
@@ -810,7 +804,7 @@
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>17</v>
@@ -819,7 +813,7 @@
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>17</v>
@@ -836,7 +830,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>17</v>
@@ -844,7 +838,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>17</v>
@@ -852,10 +846,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>21</v>
@@ -864,7 +858,7 @@
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>21</v>
@@ -872,33 +866,30 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F27" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F28" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F29" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>